<commit_message>
Move some unused Figures to Next Paper
</commit_message>
<xml_diff>
--- a/7_NematodeResearch/Fig1b_Output/TransferMatrix_EnsembleMean.xlsx
+++ b/7_NematodeResearch/Fig1b_Output/TransferMatrix_EnsembleMean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMIP6\Program\6_DrawFigure\Fig1b_Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMIP6\Program\7_NematodeResearch\Fig1b_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358782E-804C-48B5-8DA6-2B81E79688FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457EAFCC-4C57-489D-BABC-78F1C241EF44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="22845" windowHeight="13740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15270" yWindow="2520" windowWidth="27210" windowHeight="15885" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="5" r:id="rId1"/>
@@ -2137,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8988C9-F52C-4F58-B137-C5CCAEBEC674}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M28" sqref="M28:O30"/>
     </sheetView>
   </sheetViews>
@@ -2912,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EA4DFC-3DC4-4C6F-A333-4BED15F4505A}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>